<commit_message>
generacion de iva total y neto
</commit_message>
<xml_diff>
--- a/hello_world.xlsx
+++ b/hello_world.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
   <si>
     <t>Cantidad</t>
   </si>
@@ -29,6 +29,9 @@
     <t>Unitario</t>
   </si>
   <si>
+    <t>Total</t>
+  </si>
+  <si>
     <t xml:space="preserve">PALTO </t>
   </si>
   <si>
@@ -57,6 +60,12 @@
   </si>
   <si>
     <t xml:space="preserve">NETO </t>
+  </si>
+  <si>
+    <t>IVA</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
@@ -64,7 +73,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <b val="0"/>
       <i val="0"/>
@@ -72,7 +81,16 @@
       <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Century Gothic"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Century Gothic"/>
     </font>
   </fonts>
   <fills count="2">
@@ -92,8 +110,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -395,26 +416,29 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A1" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -422,10 +446,10 @@
         <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2">
         <v>4000</v>
@@ -440,10 +464,10 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3">
         <v>4000</v>
@@ -458,10 +482,10 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4">
         <v>5000</v>
@@ -476,10 +500,10 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D5">
         <v>4000</v>
@@ -494,10 +518,10 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D6">
         <v>4000</v>
@@ -512,7 +536,11 @@
       <c r="B7"/>
       <c r="C7"/>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="E7">
+        <f>E11/1.19</f>
+        <v>571428.57142857</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -520,9 +548,23 @@
       <c r="B8"/>
       <c r="C8"/>
       <c r="D8"/>
-      <c r="E8">
-        <f>A8*D8</f>
-        <v>0</v>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10">
+        <f>(E7*0.19)</f>
+        <v>108571.42857143</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11">
+        <f>SUM(E1:E6)</f>
+        <v>680000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se integra configuración de bordes
</commit_message>
<xml_diff>
--- a/hello_world.xlsx
+++ b/hello_world.xlsx
@@ -104,17 +104,53 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border/>
+    <border>
+      <left style="thick">
+        <color rgb="00000000"/>
+      </left>
+      <top style="thick">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thick">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thick">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thick">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -428,16 +464,16 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>